<commit_message>
Versión 0.75. Se agregan ejemplos por cada perfil, se corrigieron errores de redacción y de formato y se hicieron correcciones puntuales en algunos de los perfiles
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-DispensacionMedicamentoCl.xlsx
+++ b/output/StructureDefinition-DispensacionMedicamentoCl.xlsx
@@ -647,7 +647,7 @@
     <t>MedicationDispense.identifier.assigner.display</t>
   </si>
   <si>
-    <t>Se indica el nombre del dispensador que otorgo la identificacion</t>
+    <t>Se indica el nombre del dispensador que otorgo la identificación</t>
   </si>
   <si>
     <t>Plain text narrative that identifies the resource in addition to the resource reference.</t>
@@ -791,10 +791,10 @@
     <t>MedicationDispense.statusReason[x].coding.system</t>
   </si>
   <si>
-    <t>Glosa del codigo</t>
-  </si>
-  <si>
-    <t>Codigos definidos para motivos de rechazo de la dispensacion. Tabla que será generada por MINSAL</t>
+    <t>Glosa del código</t>
+  </si>
+  <si>
+    <t>Códigos definidos para motivos de rechazo de la dispensacion. Tabla que será generada por MINSAL</t>
   </si>
   <si>
     <t>Tabla que será generada por MINSAL, quedará disponible para que cada sistema la levante localmente y apunte a ella en esta ruta</t>
@@ -836,7 +836,7 @@
     <t>MedicationDispense.statusReason[x].coding.code</t>
   </si>
   <si>
-    <t>Codigo referente a la razon de porque no se entrego la dispensacion</t>
+    <t>Coódigo referente a la razon de porque no se entrego la dispensacion</t>
   </si>
   <si>
     <t>A symbol in syntax defined by the system. The symbol may be a predefined code or an expression in a syntax defined by the coding system (e.g. post-coordination).</t>
@@ -1189,7 +1189,7 @@
     <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
   </si>
   <si>
-    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should reference to some definition that establishes the system clearly and unambiguously.</t>
+    <t>Dado que estos códigos quedarán normativos y con motivo de simplificación  de desarrollo, se puede obviar la ruta *performer[Validador].function.coding.system*</t>
   </si>
   <si>
     <t>MedicationDispense.performer.function.coding.version</t>
@@ -1201,7 +1201,7 @@
     <t>Código del tipo de dispensador. Debe ser 01 para el Dispensador Obligado</t>
   </si>
   <si>
-    <t>Código del tipo de dispensador según tabla maestra. En este caso debe ser 01</t>
+    <t>Código del tipo de dispensador según tabla maestra. En este caso debe ser **Dispensador**</t>
   </si>
   <si>
     <t>MedicationDispense.performer.function.coding.display</t>
@@ -1261,10 +1261,10 @@
     <t>Función que desarrolla el Performer, en este caso validador</t>
   </si>
   <si>
-    <t>Código de validador. Debe ser 02 para definir un validador</t>
-  </si>
-  <si>
-    <t>Código de validador según tabla maestra. En este caso debe ser 02</t>
+    <t>Código de validador. Debe ser **Validador** para definir un Validador</t>
+  </si>
+  <si>
+    <t>Código de validador según tabla maestra. En este caso debe ser **Validador**</t>
   </si>
   <si>
     <t>Profesional que realiza la validación. El endPoint es ´http://api-receta.minsal.cl/v2/practitioner´</t>
@@ -1320,7 +1320,7 @@
     <t>Referencia a la prescripción que autoriza la dispensación.</t>
   </si>
   <si>
-    <t>Referencia a la prescripción que autoriza la dispensación. esta debe ser referenciada al recurso MedicarionPrescrition involucrado en la receta presentada al momento de la dspensación</t>
+    <t>Referencia a la prescripción que autoriza la dispensación. esta debe ser referenciada al recurso MedicarionRequest involucrado en la receta presentada al momento de la dspensación</t>
   </si>
   <si>
     <t>Maps to basedOn in Event logical model.</t>
@@ -1347,7 +1347,7 @@
     <t>MedicationDispense.authorizingPrescription.reference</t>
   </si>
   <si>
-    <t>Referencia a la receta que autoriza la dispensación. ´https://api-receta.minsal.cl/v2/MedicationPrescription´ (Obligada)</t>
+    <t>Referencia a la prescripción que autoriza la dispensación. ´https://api-receta.minsal.cl/v2/MedicationRequest´ (Obligada)</t>
   </si>
   <si>
     <t>Referencia a la receta que autoriza la dispensación. esta debe ser referenciada al recurso MedicarionPrescrition involucrado en la receta presentada al momento de la dspensación. ´https://api-receta.minsal.cl/v2/MediationPrescription´ (Obligada)</t>

</xml_diff>

<commit_message>
Versión 0.752, modificación menor de texto y corrección de incosistencias en los ejemplos
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-DispensacionMedicamentoCl.xlsx
+++ b/output/StructureDefinition-DispensacionMedicamentoCl.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5926" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5926" uniqueCount="681">
   <si>
     <t>Path</t>
   </si>
@@ -508,7 +508,7 @@
     <t>MedicationDispense.identifier.value</t>
   </si>
   <si>
-    <t>número identificador</t>
+    <t>Número identificador</t>
   </si>
   <si>
     <t>The portion of the identifier typically relevant to the user and which is unique within the context of the system.</t>
@@ -681,7 +681,7 @@
     <t>MedicationDispense.status</t>
   </si>
   <si>
-    <t>estado de la dispensación según estándar: cancelled | completed | entered-in-error | declined</t>
+    <t>Estado de la dispensación según estándar: cancelled | completed | entered-in-error | declined</t>
   </si>
   <si>
     <t>Estado de la dispensación, estos estaos pueden ser: preparation | in-progress | cancelled | on-hold | completed | entered-in-error | stopped | declined | unknown</t>
@@ -836,7 +836,7 @@
     <t>MedicationDispense.statusReason[x].coding.code</t>
   </si>
   <si>
-    <t>Coódigo referente a la razon de porque no se entrego la dispensacion</t>
+    <t>Código referente a la razon de porque no se entrego la dispensacion</t>
   </si>
   <si>
     <t>A symbol in syntax defined by the system. The symbol may be a predefined code or an expression in a syntax defined by the coding system (e.g. post-coordination).</t>
@@ -906,10 +906,10 @@
     <t>MedicationDispense.statusReason[x].text</t>
   </si>
   <si>
-    <t>Razon de la cancelacion. *Definir si es necesario este texto, ya que en caso de haber codificacion se puede usar display*</t>
-  </si>
-  <si>
-    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+    <t>Razon de la cancelacion</t>
+  </si>
+  <si>
+    <t>Razon de la cancelacion, explicada en texto libre</t>
   </si>
   <si>
     <t>Very often the text is the same as a displayName of one of the codings.</t>
@@ -1074,7 +1074,7 @@
     <t>Profesional que realizó la orden.</t>
   </si>
   <si>
-    <t>Indicates who or what performed the event.</t>
+    <t>Profesional que realizó o validó la entrega de la orden de fármacos.</t>
   </si>
   <si>
     <t>Se definen dos tipos de dispensador, no excluyentes mutuamente. El primero es el dispensador del fármaco pero el segundo es el validador. El dispensador es obligado. Ambos son iguales desde el punto de vista del desarrollo de cada slice es el mismo solo debe cambiar el valor del código del la ruta performer.function.code</t>
@@ -1201,7 +1201,7 @@
     <t>Código del tipo de dispensador. Debe ser 01 para el Dispensador Obligado</t>
   </si>
   <si>
-    <t>Código del tipo de dispensador según tabla maestra. En este caso debe ser **Dispensador**</t>
+    <t>Código del tipo de dispensador según tabla maestra. En este caso debe ser Dispensador</t>
   </si>
   <si>
     <t>MedicationDispense.performer.function.coding.display</t>
@@ -1216,6 +1216,9 @@
     <t>Plain text representation of the concept</t>
   </si>
   <si>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
     <t>Profesional que realiza la dispensación. El endPoint es ´http://api-receta.minsal.cl/v2/practitioner´</t>
   </si>
   <si>
@@ -1255,7 +1258,7 @@
     <t>Se entiende por dispensador al individuo que valida la entrega los medicamentos a quien los solicite en el punto de entrega. Por lo común es un Químico Farmaceutico de Profesión</t>
   </si>
   <si>
-    <t>Función que desarrolla el Validador, en este caso siempre será un QF</t>
+    <t>Función que desarrolla el Validador, en este caso siempre será un Químico Farmaceutico</t>
   </si>
   <si>
     <t>Función que desarrolla el Performer, en este caso validador</t>
@@ -1264,7 +1267,7 @@
     <t>Código de validador. Debe ser **Validador** para definir un Validador</t>
   </si>
   <si>
-    <t>Código de validador según tabla maestra. En este caso debe ser **Validador**</t>
+    <t>Código de validador según tabla maestra. En este caso debe ser Validador</t>
   </si>
   <si>
     <t>Profesional que realiza la validación. El endPoint es ´http://api-receta.minsal.cl/v2/practitioner´</t>
@@ -1320,7 +1323,7 @@
     <t>Referencia a la prescripción que autoriza la dispensación.</t>
   </si>
   <si>
-    <t>Referencia a la prescripción que autoriza la dispensación. esta debe ser referenciada al recurso MedicarionRequest involucrado en la receta presentada al momento de la dspensación</t>
+    <t>Referencia a la prescripción que autoriza la dispensación. Esta debe ser referenciada al recurso MedicarionRequest involucrado en la receta presentada al momento de la dspensación</t>
   </si>
   <si>
     <t>Maps to basedOn in Event logical model.</t>
@@ -1608,9 +1611,6 @@
     <t>Instruccion de dosificación</t>
   </si>
   <si>
-    <t>Free text dosage instructions e.g. SIG.</t>
-  </si>
-  <si>
     <t>Free text dosage instructions can be used for cases where the instructions are too complex to code.  The content of this attribute does not include the name or description of the medication. When coded instructions are present, the free text instructions may still be present for display to humans taking or administering the medication. It is expected that the text instructions will always be populated.  If the dosage.timing attribute is also populated, then the dosage.text should reflect the same information as the timing.  Additional information about administration or preparation of the medication should be included as text.</t>
   </si>
   <si>
@@ -1624,9 +1624,6 @@
   </si>
   <si>
     <t>Instrucciones, advertencias y/o efectos secundarios</t>
-  </si>
-  <si>
-    <t>Supplemental instructions to the patient on how to take the medication  (e.g. "with meals" or"take half to one hour before food") or warnings for the patient about the medication (e.g. "may cause drowsiness" or "avoid exposure of skin to direct sunlight or sunlamps").</t>
   </si>
   <si>
     <t>Information about administration or preparation of the medication (e.g. "infuse as rapidly as possibly via intraperitoneal port" or "immediately following drug x") should be populated in dosage.text.</t>
@@ -1669,9 +1666,6 @@
     <t>Cuando se debe administrar los medicamentos</t>
   </si>
   <si>
-    <t>When medication should be administered.</t>
-  </si>
-  <si>
     <t>This attribute might not always be populated while the Dosage.text is expected to be populated.  If both are populated, then the Dosage.text should reflect the content of the Dosage.timing.</t>
   </si>
   <si>
@@ -1708,7 +1702,10 @@
     <t>asNeededBoolean</t>
   </si>
   <si>
-    <t>En caso de SOS, se usa, considerar este valor como booleano</t>
+    <t>Se define para uso de fármaco sin receta o indicación en esta.</t>
+  </si>
+  <si>
+    <t>Para indicar si el fármaco se puede usar sin respetar diretamente lo presctito en el dosaje, como por ejemplo medicamentos que se pueden usar en caso de SOS</t>
   </si>
   <si>
     <t>MedicationDispense.dosageInstruction.site</t>
@@ -1747,9 +1744,6 @@
     <t>Como se debe administrar el medicamento (Via de administración o como debe el farmaco entrar al cuerpo)</t>
   </si>
   <si>
-    <t>How drug should enter body.</t>
-  </si>
-  <si>
     <t>A code specifying the route or physiological path of administration of a therapeutic agent into or onto a patient's body.</t>
   </si>
   <si>
@@ -1771,7 +1765,7 @@
     <t>MedicationDispense.dosageInstruction.method</t>
   </si>
   <si>
-    <t>Tecnica para administrar el medicamento</t>
+    <t>Técnica para administrar el medicamento</t>
   </si>
   <si>
     <t>Es un valor codificado que indica el método mediante el cual se introduce el medicamento en el cuerpo o sobre él. Más comúnmente utilizado para inyecciones. Por ejemplo, empuje lento; Profundo IV.</t>
@@ -1806,9 +1800,6 @@
   </si>
   <si>
     <t>Cantidad de los medicamentos a administrar</t>
-  </si>
-  <si>
-    <t>The amount of medication administered.</t>
   </si>
   <si>
     <t>Dosage.doseAndRate</t>
@@ -9993,7 +9984,7 @@
         <v>386</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>288</v>
+        <v>387</v>
       </c>
       <c r="M68" t="s" s="2">
         <v>289</v>
@@ -10106,7 +10097,7 @@
         <v>361</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="L69" t="s" s="2">
         <v>363</v>
@@ -10192,7 +10183,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -10304,7 +10295,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -10418,7 +10409,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -10444,10 +10435,10 @@
         <v>52</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M72" t="s" s="2">
         <v>185</v>
@@ -10532,7 +10523,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -10646,7 +10637,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10760,7 +10751,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -10786,7 +10777,7 @@
         <v>52</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L75" t="s" s="2">
         <v>203</v>
@@ -10877,7 +10868,7 @@
         <v>337</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C76" t="s" s="2">
         <v>41</v>
@@ -10902,10 +10893,10 @@
         <v>339</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -11356,10 +11347,10 @@
         <v>138</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" t="s" s="2">
@@ -12268,10 +12259,10 @@
         <v>70</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" t="s" s="2">
@@ -12285,7 +12276,7 @@
         <v>41</v>
       </c>
       <c r="R88" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="S88" t="s" s="2">
         <v>41</v>
@@ -12615,7 +12606,7 @@
         <v>386</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>288</v>
+        <v>387</v>
       </c>
       <c r="M91" t="s" s="2">
         <v>289</v>
@@ -12728,7 +12719,7 @@
         <v>361</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L92" t="s" s="2">
         <v>363</v>
@@ -12814,7 +12805,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -12926,7 +12917,7 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
@@ -13040,7 +13031,7 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
@@ -13066,10 +13057,10 @@
         <v>52</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M95" t="s" s="2">
         <v>185</v>
@@ -13154,7 +13145,7 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -13268,7 +13259,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -13382,7 +13373,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -13408,7 +13399,7 @@
         <v>52</v>
       </c>
       <c r="K98" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L98" t="s" s="2">
         <v>203</v>
@@ -13496,7 +13487,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -13519,13 +13510,13 @@
         <v>41</v>
       </c>
       <c r="J99" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="K99" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="L99" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -13576,7 +13567,7 @@
         <v>41</v>
       </c>
       <c r="AE99" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AF99" t="s" s="2">
         <v>42</v>
@@ -13594,7 +13585,7 @@
         <v>41</v>
       </c>
       <c r="AK99" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AL99" t="s" s="2">
         <v>41</v>
@@ -13608,7 +13599,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -13720,7 +13711,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -13834,7 +13825,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -13860,10 +13851,10 @@
         <v>52</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M102" t="s" s="2">
         <v>185</v>
@@ -13948,7 +13939,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -14062,7 +14053,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -14176,7 +14167,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -14202,7 +14193,7 @@
         <v>52</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L105" t="s" s="2">
         <v>203</v>
@@ -14290,7 +14281,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -14313,16 +14304,16 @@
         <v>41</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="M106" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="N106" s="2"/>
       <c r="O106" t="s" s="2">
@@ -14372,7 +14363,7 @@
         <v>41</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AF106" t="s" s="2">
         <v>42</v>
@@ -14387,24 +14378,24 @@
         <v>62</v>
       </c>
       <c r="AJ106" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AK106" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="AL106" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM106" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AN106" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -14516,7 +14507,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -14630,7 +14621,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -14656,10 +14647,10 @@
         <v>52</v>
       </c>
       <c r="K109" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="M109" t="s" s="2">
         <v>185</v>
@@ -14744,7 +14735,7 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -14858,7 +14849,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -14972,7 +14963,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -14998,7 +14989,7 @@
         <v>52</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L112" t="s" s="2">
         <v>203</v>
@@ -15086,7 +15077,7 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -15112,10 +15103,10 @@
         <v>138</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
@@ -15145,10 +15136,10 @@
         <v>225</v>
       </c>
       <c r="X113" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="Y113" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="Z113" t="s" s="2">
         <v>41</v>
@@ -15166,7 +15157,7 @@
         <v>41</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>42</v>
@@ -15184,21 +15175,21 @@
         <v>41</v>
       </c>
       <c r="AK113" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AL113" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM113" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AN113" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -15221,13 +15212,13 @@
         <v>41</v>
       </c>
       <c r="J114" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="K114" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="L114" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
@@ -15278,7 +15269,7 @@
         <v>41</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>42</v>
@@ -15296,21 +15287,21 @@
         <v>41</v>
       </c>
       <c r="AK114" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AL114" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM114" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AN114" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" t="s" s="2">
@@ -15333,13 +15324,13 @@
         <v>41</v>
       </c>
       <c r="J115" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="K115" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="L115" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
@@ -15390,7 +15381,7 @@
         <v>41</v>
       </c>
       <c r="AE115" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AF115" t="s" s="2">
         <v>42</v>
@@ -15408,7 +15399,7 @@
         <v>41</v>
       </c>
       <c r="AK115" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AL115" t="s" s="2">
         <v>41</v>
@@ -15417,12 +15408,12 @@
         <v>41</v>
       </c>
       <c r="AN115" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" t="s" s="2">
@@ -15445,13 +15436,13 @@
         <v>51</v>
       </c>
       <c r="J116" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="L116" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
@@ -15502,7 +15493,7 @@
         <v>41</v>
       </c>
       <c r="AE116" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AF116" t="s" s="2">
         <v>42</v>
@@ -15520,21 +15511,21 @@
         <v>41</v>
       </c>
       <c r="AK116" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="AL116" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM116" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="AN116" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
@@ -15557,16 +15548,16 @@
         <v>41</v>
       </c>
       <c r="J117" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K117" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="L117" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="M117" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="N117" s="2"/>
       <c r="O117" t="s" s="2">
@@ -15616,7 +15607,7 @@
         <v>41</v>
       </c>
       <c r="AE117" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AF117" t="s" s="2">
         <v>42</v>
@@ -15631,24 +15622,24 @@
         <v>62</v>
       </c>
       <c r="AJ117" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AK117" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AL117" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM117" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="AN117" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -15671,13 +15662,13 @@
         <v>41</v>
       </c>
       <c r="J118" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="K118" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="L118" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
@@ -15728,7 +15719,7 @@
         <v>41</v>
       </c>
       <c r="AE118" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AF118" t="s" s="2">
         <v>42</v>
@@ -15746,21 +15737,21 @@
         <v>41</v>
       </c>
       <c r="AK118" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="AL118" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM118" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AN118" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" t="s" s="2">
@@ -15783,13 +15774,13 @@
         <v>41</v>
       </c>
       <c r="J119" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="K119" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="L119" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
@@ -15840,7 +15831,7 @@
         <v>41</v>
       </c>
       <c r="AE119" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AF119" t="s" s="2">
         <v>42</v>
@@ -15858,13 +15849,13 @@
         <v>41</v>
       </c>
       <c r="AK119" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AL119" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM119" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AN119" t="s" s="2">
         <v>41</v>
@@ -15872,7 +15863,7 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" t="s" s="2">
@@ -15984,7 +15975,7 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" t="s" s="2">
@@ -16098,7 +16089,7 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" t="s" s="2">
@@ -16212,7 +16203,7 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" t="s" s="2">
@@ -16326,7 +16317,7 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" t="s" s="2">
@@ -16440,7 +16431,7 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" t="s" s="2">
@@ -16466,13 +16457,13 @@
         <v>52</v>
       </c>
       <c r="K125" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L125" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="M125" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="N125" s="2"/>
       <c r="O125" t="s" s="2">
@@ -16554,7 +16545,7 @@
     </row>
     <row r="126">
       <c r="A126" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" t="s" s="2">
@@ -16577,13 +16568,13 @@
         <v>41</v>
       </c>
       <c r="J126" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="K126" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="L126" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
@@ -16634,7 +16625,7 @@
         <v>41</v>
       </c>
       <c r="AE126" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="AF126" t="s" s="2">
         <v>42</v>
@@ -16649,10 +16640,10 @@
         <v>62</v>
       </c>
       <c r="AJ126" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="AK126" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="AL126" t="s" s="2">
         <v>41</v>
@@ -16661,12 +16652,12 @@
         <v>41</v>
       </c>
       <c r="AN126" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -16689,16 +16680,16 @@
         <v>41</v>
       </c>
       <c r="J127" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="K127" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="L127" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="M127" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="N127" s="2"/>
       <c r="O127" t="s" s="2">
@@ -16748,7 +16739,7 @@
         <v>41</v>
       </c>
       <c r="AE127" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AF127" t="s" s="2">
         <v>42</v>
@@ -16766,7 +16757,7 @@
         <v>41</v>
       </c>
       <c r="AK127" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AL127" t="s" s="2">
         <v>41</v>
@@ -16780,7 +16771,7 @@
     </row>
     <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -16892,7 +16883,7 @@
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" t="s" s="2">
@@ -17006,7 +16997,7 @@
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" t="s" s="2">
@@ -17122,7 +17113,7 @@
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" t="s" s="2">
@@ -17145,17 +17136,17 @@
         <v>51</v>
       </c>
       <c r="J131" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="K131" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="L131" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="M131" s="2"/>
       <c r="N131" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="O131" t="s" s="2">
         <v>41</v>
@@ -17204,7 +17195,7 @@
         <v>41</v>
       </c>
       <c r="AE131" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="AF131" t="s" s="2">
         <v>42</v>
@@ -17222,7 +17213,7 @@
         <v>41</v>
       </c>
       <c r="AK131" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="AL131" t="s" s="2">
         <v>41</v>
@@ -17231,12 +17222,12 @@
         <v>41</v>
       </c>
       <c r="AN131" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" t="s" s="2">
@@ -17262,7 +17253,7 @@
         <v>52</v>
       </c>
       <c r="K132" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="L132" t="s" s="2">
         <v>514</v>
@@ -17336,7 +17327,7 @@
         <v>41</v>
       </c>
       <c r="AK132" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="AL132" t="s" s="2">
         <v>41</v>
@@ -17379,13 +17370,13 @@
         <v>519</v>
       </c>
       <c r="L133" t="s" s="2">
+        <v>519</v>
+      </c>
+      <c r="M133" t="s" s="2">
         <v>520</v>
       </c>
-      <c r="M133" t="s" s="2">
+      <c r="N133" t="s" s="2">
         <v>521</v>
-      </c>
-      <c r="N133" t="s" s="2">
-        <v>522</v>
       </c>
       <c r="O133" t="s" s="2">
         <v>41</v>
@@ -17413,28 +17404,28 @@
         <v>225</v>
       </c>
       <c r="X133" t="s" s="2">
+        <v>522</v>
+      </c>
+      <c r="Y133" t="s" s="2">
         <v>523</v>
       </c>
-      <c r="Y133" t="s" s="2">
+      <c r="Z133" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA133" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB133" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC133" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD133" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE133" t="s" s="2">
         <v>524</v>
-      </c>
-      <c r="Z133" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA133" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB133" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC133" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD133" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE133" t="s" s="2">
-        <v>525</v>
       </c>
       <c r="AF133" t="s" s="2">
         <v>42</v>
@@ -17452,7 +17443,7 @@
         <v>41</v>
       </c>
       <c r="AK133" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="AL133" t="s" s="2">
         <v>41</v>
@@ -17461,12 +17452,12 @@
         <v>41</v>
       </c>
       <c r="AN133" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" t="s" s="2">
@@ -17492,10 +17483,10 @@
         <v>52</v>
       </c>
       <c r="K134" t="s" s="2">
+        <v>527</v>
+      </c>
+      <c r="L134" t="s" s="2">
         <v>528</v>
-      </c>
-      <c r="L134" t="s" s="2">
-        <v>529</v>
       </c>
       <c r="M134" s="2"/>
       <c r="N134" s="2"/>
@@ -17546,7 +17537,7 @@
         <v>41</v>
       </c>
       <c r="AE134" t="s" s="2">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AF134" t="s" s="2">
         <v>42</v>
@@ -17564,7 +17555,7 @@
         <v>41</v>
       </c>
       <c r="AK134" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="AL134" t="s" s="2">
         <v>41</v>
@@ -17573,12 +17564,12 @@
         <v>41</v>
       </c>
       <c r="AN134" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="135" hidden="true">
       <c r="A135" t="s" s="2">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" t="s" s="2">
@@ -17601,19 +17592,19 @@
         <v>51</v>
       </c>
       <c r="J135" t="s" s="2">
+        <v>531</v>
+      </c>
+      <c r="K135" t="s" s="2">
         <v>532</v>
       </c>
-      <c r="K135" t="s" s="2">
+      <c r="L135" t="s" s="2">
+        <v>532</v>
+      </c>
+      <c r="M135" t="s" s="2">
         <v>533</v>
       </c>
-      <c r="L135" t="s" s="2">
+      <c r="N135" t="s" s="2">
         <v>534</v>
-      </c>
-      <c r="M135" t="s" s="2">
-        <v>535</v>
-      </c>
-      <c r="N135" t="s" s="2">
-        <v>536</v>
       </c>
       <c r="O135" t="s" s="2">
         <v>41</v>
@@ -17662,7 +17653,7 @@
         <v>41</v>
       </c>
       <c r="AE135" t="s" s="2">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AF135" t="s" s="2">
         <v>42</v>
@@ -17680,7 +17671,7 @@
         <v>41</v>
       </c>
       <c r="AK135" t="s" s="2">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="AL135" t="s" s="2">
         <v>41</v>
@@ -17694,7 +17685,7 @@
     </row>
     <row r="136" hidden="true">
       <c r="A136" t="s" s="2">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" t="s" s="2">
@@ -17720,13 +17711,13 @@
         <v>278</v>
       </c>
       <c r="K136" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="L136" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="M136" t="s" s="2">
         <v>540</v>
-      </c>
-      <c r="L136" t="s" s="2">
-        <v>541</v>
-      </c>
-      <c r="M136" t="s" s="2">
-        <v>542</v>
       </c>
       <c r="N136" s="2"/>
       <c r="O136" t="s" s="2">
@@ -17774,7 +17765,7 @@
         <v>229</v>
       </c>
       <c r="AE136" t="s" s="2">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="AF136" t="s" s="2">
         <v>42</v>
@@ -17792,7 +17783,7 @@
         <v>41</v>
       </c>
       <c r="AK136" t="s" s="2">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="AL136" t="s" s="2">
         <v>41</v>
@@ -17801,15 +17792,15 @@
         <v>41</v>
       </c>
       <c r="AN136" t="s" s="2">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="137" hidden="true">
       <c r="A137" t="s" s="2">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B137" t="s" s="2">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C137" t="s" s="2">
         <v>41</v>
@@ -17834,13 +17825,13 @@
         <v>278</v>
       </c>
       <c r="K137" t="s" s="2">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L137" t="s" s="2">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="M137" t="s" s="2">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="N137" s="2"/>
       <c r="O137" t="s" s="2">
@@ -17890,7 +17881,7 @@
         <v>41</v>
       </c>
       <c r="AE137" t="s" s="2">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="AF137" t="s" s="2">
         <v>42</v>
@@ -17908,7 +17899,7 @@
         <v>41</v>
       </c>
       <c r="AK137" t="s" s="2">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="AL137" t="s" s="2">
         <v>41</v>
@@ -17917,12 +17908,12 @@
         <v>41</v>
       </c>
       <c r="AN137" t="s" s="2">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="138" hidden="true">
       <c r="A138" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" t="s" s="2">
@@ -17948,16 +17939,16 @@
         <v>138</v>
       </c>
       <c r="K138" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="L138" t="s" s="2">
         <v>549</v>
       </c>
-      <c r="L138" t="s" s="2">
+      <c r="M138" t="s" s="2">
         <v>550</v>
       </c>
-      <c r="M138" t="s" s="2">
+      <c r="N138" t="s" s="2">
         <v>551</v>
-      </c>
-      <c r="N138" t="s" s="2">
-        <v>552</v>
       </c>
       <c r="O138" t="s" s="2">
         <v>41</v>
@@ -17985,28 +17976,28 @@
         <v>225</v>
       </c>
       <c r="X138" t="s" s="2">
+        <v>552</v>
+      </c>
+      <c r="Y138" t="s" s="2">
         <v>553</v>
       </c>
-      <c r="Y138" t="s" s="2">
+      <c r="Z138" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA138" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB138" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC138" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD138" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE138" t="s" s="2">
         <v>554</v>
-      </c>
-      <c r="Z138" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA138" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB138" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC138" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD138" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE138" t="s" s="2">
-        <v>555</v>
       </c>
       <c r="AF138" t="s" s="2">
         <v>42</v>
@@ -18024,21 +18015,21 @@
         <v>41</v>
       </c>
       <c r="AK138" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="AL138" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AM138" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN138" t="s" s="2">
         <v>556</v>
-      </c>
-      <c r="AL138" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AM138" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AN138" t="s" s="2">
-        <v>557</v>
       </c>
     </row>
     <row r="139" hidden="true">
       <c r="A139" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" t="s" s="2">
@@ -18064,14 +18055,14 @@
         <v>138</v>
       </c>
       <c r="K139" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="L139" t="s" s="2">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="M139" s="2"/>
       <c r="N139" t="s" s="2">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="O139" t="s" s="2">
         <v>41</v>
@@ -18099,28 +18090,28 @@
         <v>225</v>
       </c>
       <c r="X139" t="s" s="2">
+        <v>560</v>
+      </c>
+      <c r="Y139" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="Z139" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA139" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB139" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC139" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD139" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE139" t="s" s="2">
         <v>562</v>
-      </c>
-      <c r="Y139" t="s" s="2">
-        <v>563</v>
-      </c>
-      <c r="Z139" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA139" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB139" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC139" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD139" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE139" t="s" s="2">
-        <v>564</v>
       </c>
       <c r="AF139" t="s" s="2">
         <v>42</v>
@@ -18138,7 +18129,7 @@
         <v>41</v>
       </c>
       <c r="AK139" t="s" s="2">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AL139" t="s" s="2">
         <v>41</v>
@@ -18147,12 +18138,12 @@
         <v>41</v>
       </c>
       <c r="AN139" t="s" s="2">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="140" hidden="true">
       <c r="A140" t="s" s="2">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" t="s" s="2">
@@ -18178,16 +18169,16 @@
         <v>138</v>
       </c>
       <c r="K140" t="s" s="2">
+        <v>566</v>
+      </c>
+      <c r="L140" t="s" s="2">
+        <v>567</v>
+      </c>
+      <c r="M140" t="s" s="2">
         <v>568</v>
       </c>
-      <c r="L140" t="s" s="2">
+      <c r="N140" t="s" s="2">
         <v>569</v>
-      </c>
-      <c r="M140" t="s" s="2">
-        <v>570</v>
-      </c>
-      <c r="N140" t="s" s="2">
-        <v>571</v>
       </c>
       <c r="O140" t="s" s="2">
         <v>41</v>
@@ -18215,28 +18206,28 @@
         <v>225</v>
       </c>
       <c r="X140" t="s" s="2">
+        <v>570</v>
+      </c>
+      <c r="Y140" t="s" s="2">
+        <v>571</v>
+      </c>
+      <c r="Z140" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA140" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB140" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC140" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD140" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE140" t="s" s="2">
         <v>572</v>
-      </c>
-      <c r="Y140" t="s" s="2">
-        <v>573</v>
-      </c>
-      <c r="Z140" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA140" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB140" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC140" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD140" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE140" t="s" s="2">
-        <v>574</v>
       </c>
       <c r="AF140" t="s" s="2">
         <v>42</v>
@@ -18254,7 +18245,7 @@
         <v>41</v>
       </c>
       <c r="AK140" t="s" s="2">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="AL140" t="s" s="2">
         <v>41</v>
@@ -18263,12 +18254,12 @@
         <v>41</v>
       </c>
       <c r="AN140" t="s" s="2">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="141" hidden="true">
       <c r="A141" t="s" s="2">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" t="s" s="2">
@@ -18291,13 +18282,13 @@
         <v>51</v>
       </c>
       <c r="J141" t="s" s="2">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="K141" t="s" s="2">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="L141" t="s" s="2">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="M141" s="2"/>
       <c r="N141" s="2"/>
@@ -18348,7 +18339,7 @@
         <v>41</v>
       </c>
       <c r="AE141" t="s" s="2">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="AF141" t="s" s="2">
         <v>42</v>
@@ -18375,12 +18366,12 @@
         <v>41</v>
       </c>
       <c r="AN141" t="s" s="2">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="142" hidden="true">
       <c r="A142" t="s" s="2">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" t="s" s="2">
@@ -18492,7 +18483,7 @@
     </row>
     <row r="143" hidden="true">
       <c r="A143" t="s" s="2">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -18606,7 +18597,7 @@
     </row>
     <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
@@ -18632,14 +18623,14 @@
         <v>138</v>
       </c>
       <c r="K144" t="s" s="2">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="L144" t="s" s="2">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="M144" s="2"/>
       <c r="N144" t="s" s="2">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="O144" t="s" s="2">
         <v>41</v>
@@ -18667,10 +18658,10 @@
         <v>225</v>
       </c>
       <c r="X144" t="s" s="2">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="Y144" t="s" s="2">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="Z144" t="s" s="2">
         <v>41</v>
@@ -18688,7 +18679,7 @@
         <v>41</v>
       </c>
       <c r="AE144" t="s" s="2">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="AF144" t="s" s="2">
         <v>42</v>
@@ -18715,12 +18706,12 @@
         <v>41</v>
       </c>
       <c r="AN144" t="s" s="2">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -18743,19 +18734,19 @@
         <v>51</v>
       </c>
       <c r="J145" t="s" s="2">
+        <v>591</v>
+      </c>
+      <c r="K145" t="s" s="2">
+        <v>592</v>
+      </c>
+      <c r="L145" t="s" s="2">
+        <v>593</v>
+      </c>
+      <c r="M145" t="s" s="2">
         <v>594</v>
       </c>
-      <c r="K145" t="s" s="2">
+      <c r="N145" t="s" s="2">
         <v>595</v>
-      </c>
-      <c r="L145" t="s" s="2">
-        <v>596</v>
-      </c>
-      <c r="M145" t="s" s="2">
-        <v>597</v>
-      </c>
-      <c r="N145" t="s" s="2">
-        <v>598</v>
       </c>
       <c r="O145" t="s" s="2">
         <v>41</v>
@@ -18804,7 +18795,7 @@
         <v>41</v>
       </c>
       <c r="AE145" t="s" s="2">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="AF145" t="s" s="2">
         <v>42</v>
@@ -18822,7 +18813,7 @@
         <v>41</v>
       </c>
       <c r="AK145" t="s" s="2">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="AL145" t="s" s="2">
         <v>41</v>
@@ -18831,12 +18822,12 @@
         <v>41</v>
       </c>
       <c r="AN145" t="s" s="2">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="146" hidden="true">
       <c r="A146" t="s" s="2">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" t="s" s="2">
@@ -18859,19 +18850,19 @@
         <v>51</v>
       </c>
       <c r="J146" t="s" s="2">
+        <v>599</v>
+      </c>
+      <c r="K146" t="s" s="2">
+        <v>600</v>
+      </c>
+      <c r="L146" t="s" s="2">
+        <v>601</v>
+      </c>
+      <c r="M146" t="s" s="2">
         <v>602</v>
       </c>
-      <c r="K146" t="s" s="2">
+      <c r="N146" t="s" s="2">
         <v>603</v>
-      </c>
-      <c r="L146" t="s" s="2">
-        <v>604</v>
-      </c>
-      <c r="M146" t="s" s="2">
-        <v>605</v>
-      </c>
-      <c r="N146" t="s" s="2">
-        <v>606</v>
       </c>
       <c r="O146" t="s" s="2">
         <v>41</v>
@@ -18920,7 +18911,7 @@
         <v>41</v>
       </c>
       <c r="AE146" t="s" s="2">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="AF146" t="s" s="2">
         <v>42</v>
@@ -18938,7 +18929,7 @@
         <v>41</v>
       </c>
       <c r="AK146" t="s" s="2">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AL146" t="s" s="2">
         <v>41</v>
@@ -18947,12 +18938,12 @@
         <v>41</v>
       </c>
       <c r="AN146" t="s" s="2">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" t="s" s="2">
@@ -18975,19 +18966,19 @@
         <v>51</v>
       </c>
       <c r="J147" t="s" s="2">
+        <v>608</v>
+      </c>
+      <c r="K147" t="s" s="2">
+        <v>609</v>
+      </c>
+      <c r="L147" t="s" s="2">
+        <v>610</v>
+      </c>
+      <c r="M147" t="s" s="2">
         <v>611</v>
       </c>
-      <c r="K147" t="s" s="2">
+      <c r="N147" t="s" s="2">
         <v>612</v>
-      </c>
-      <c r="L147" t="s" s="2">
-        <v>613</v>
-      </c>
-      <c r="M147" t="s" s="2">
-        <v>614</v>
-      </c>
-      <c r="N147" t="s" s="2">
-        <v>615</v>
       </c>
       <c r="O147" t="s" s="2">
         <v>41</v>
@@ -19036,7 +19027,7 @@
         <v>41</v>
       </c>
       <c r="AE147" t="s" s="2">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AF147" t="s" s="2">
         <v>42</v>
@@ -19054,7 +19045,7 @@
         <v>41</v>
       </c>
       <c r="AK147" t="s" s="2">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="AL147" t="s" s="2">
         <v>41</v>
@@ -19063,12 +19054,12 @@
         <v>41</v>
       </c>
       <c r="AN147" t="s" s="2">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="148" hidden="true">
       <c r="A148" t="s" s="2">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" t="s" s="2">
@@ -19091,19 +19082,19 @@
         <v>51</v>
       </c>
       <c r="J148" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="K148" t="s" s="2">
+        <v>617</v>
+      </c>
+      <c r="L148" t="s" s="2">
+        <v>618</v>
+      </c>
+      <c r="M148" t="s" s="2">
+        <v>619</v>
+      </c>
+      <c r="N148" t="s" s="2">
         <v>620</v>
-      </c>
-      <c r="L148" t="s" s="2">
-        <v>621</v>
-      </c>
-      <c r="M148" t="s" s="2">
-        <v>622</v>
-      </c>
-      <c r="N148" t="s" s="2">
-        <v>623</v>
       </c>
       <c r="O148" t="s" s="2">
         <v>41</v>
@@ -19152,7 +19143,7 @@
         <v>41</v>
       </c>
       <c r="AE148" t="s" s="2">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="AF148" t="s" s="2">
         <v>42</v>
@@ -19170,7 +19161,7 @@
         <v>41</v>
       </c>
       <c r="AK148" t="s" s="2">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="AL148" t="s" s="2">
         <v>41</v>
@@ -19184,7 +19175,7 @@
     </row>
     <row r="149" hidden="true">
       <c r="A149" t="s" s="2">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" t="s" s="2">
@@ -19207,17 +19198,17 @@
         <v>51</v>
       </c>
       <c r="J149" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="K149" t="s" s="2">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="L149" t="s" s="2">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="M149" s="2"/>
       <c r="N149" t="s" s="2">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="O149" t="s" s="2">
         <v>41</v>
@@ -19266,7 +19257,7 @@
         <v>41</v>
       </c>
       <c r="AE149" t="s" s="2">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="AF149" t="s" s="2">
         <v>42</v>
@@ -19284,7 +19275,7 @@
         <v>41</v>
       </c>
       <c r="AK149" t="s" s="2">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="AL149" t="s" s="2">
         <v>41</v>
@@ -19298,7 +19289,7 @@
     </row>
     <row r="150" hidden="true">
       <c r="A150" t="s" s="2">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" t="s" s="2">
@@ -19324,10 +19315,10 @@
         <v>339</v>
       </c>
       <c r="K150" t="s" s="2">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
@@ -19378,7 +19369,7 @@
         <v>41</v>
       </c>
       <c r="AE150" t="s" s="2">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="AF150" t="s" s="2">
         <v>42</v>
@@ -19396,13 +19387,13 @@
         <v>41</v>
       </c>
       <c r="AK150" t="s" s="2">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="AL150" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM150" t="s" s="2">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="AN150" t="s" s="2">
         <v>41</v>
@@ -19410,7 +19401,7 @@
     </row>
     <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" t="s" s="2">
@@ -19522,7 +19513,7 @@
     </row>
     <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" t="s" s="2">
@@ -19636,7 +19627,7 @@
     </row>
     <row r="153" hidden="true">
       <c r="A153" t="s" s="2">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" t="s" s="2">
@@ -19752,7 +19743,7 @@
     </row>
     <row r="154" hidden="true">
       <c r="A154" t="s" s="2">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" t="s" s="2">
@@ -19778,10 +19769,10 @@
         <v>278</v>
       </c>
       <c r="K154" t="s" s="2">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="L154" t="s" s="2">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
@@ -19832,7 +19823,7 @@
         <v>41</v>
       </c>
       <c r="AE154" t="s" s="2">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="AF154" t="s" s="2">
         <v>50</v>
@@ -19850,7 +19841,7 @@
         <v>41</v>
       </c>
       <c r="AK154" t="s" s="2">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="AL154" t="s" s="2">
         <v>41</v>
@@ -19864,7 +19855,7 @@
     </row>
     <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" t="s" s="2">
@@ -19890,10 +19881,10 @@
         <v>138</v>
       </c>
       <c r="K155" t="s" s="2">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="L155" t="s" s="2">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="M155" s="2"/>
       <c r="N155" s="2"/>
@@ -19923,10 +19914,10 @@
         <v>225</v>
       </c>
       <c r="X155" t="s" s="2">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="Y155" t="s" s="2">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="Z155" t="s" s="2">
         <v>41</v>
@@ -19944,7 +19935,7 @@
         <v>41</v>
       </c>
       <c r="AE155" t="s" s="2">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="AF155" t="s" s="2">
         <v>42</v>
@@ -19962,21 +19953,21 @@
         <v>41</v>
       </c>
       <c r="AK155" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AL155" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM155" t="s" s="2">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="AN155" t="s" s="2">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="156" hidden="true">
       <c r="A156" t="s" s="2">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" t="s" s="2">
@@ -20002,10 +19993,10 @@
         <v>138</v>
       </c>
       <c r="K156" t="s" s="2">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="L156" t="s" s="2">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
@@ -20035,10 +20026,10 @@
         <v>225</v>
       </c>
       <c r="X156" t="s" s="2">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="Y156" t="s" s="2">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="Z156" t="s" s="2">
         <v>41</v>
@@ -20056,7 +20047,7 @@
         <v>41</v>
       </c>
       <c r="AE156" t="s" s="2">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="AF156" t="s" s="2">
         <v>42</v>
@@ -20074,13 +20065,13 @@
         <v>41</v>
       </c>
       <c r="AK156" t="s" s="2">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="AL156" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM156" t="s" s="2">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="AN156" t="s" s="2">
         <v>41</v>
@@ -20088,7 +20079,7 @@
     </row>
     <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" t="s" s="2">
@@ -20111,13 +20102,13 @@
         <v>41</v>
       </c>
       <c r="J157" t="s" s="2">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="K157" t="s" s="2">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="L157" t="s" s="2">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
@@ -20168,7 +20159,7 @@
         <v>41</v>
       </c>
       <c r="AE157" t="s" s="2">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="AF157" t="s" s="2">
         <v>42</v>
@@ -20186,13 +20177,13 @@
         <v>41</v>
       </c>
       <c r="AK157" t="s" s="2">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="AL157" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AM157" t="s" s="2">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="AN157" t="s" s="2">
         <v>41</v>
@@ -20200,11 +20191,11 @@
     </row>
     <row r="158">
       <c r="A158" t="s" s="2">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" t="s" s="2">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D158" s="2"/>
       <c r="E158" t="s" s="2">
@@ -20223,16 +20214,16 @@
         <v>41</v>
       </c>
       <c r="J158" t="s" s="2">
+        <v>662</v>
+      </c>
+      <c r="K158" t="s" s="2">
+        <v>663</v>
+      </c>
+      <c r="L158" t="s" s="2">
+        <v>664</v>
+      </c>
+      <c r="M158" t="s" s="2">
         <v>665</v>
-      </c>
-      <c r="K158" t="s" s="2">
-        <v>666</v>
-      </c>
-      <c r="L158" t="s" s="2">
-        <v>667</v>
-      </c>
-      <c r="M158" t="s" s="2">
-        <v>668</v>
       </c>
       <c r="N158" s="2"/>
       <c r="O158" t="s" s="2">
@@ -20282,7 +20273,7 @@
         <v>41</v>
       </c>
       <c r="AE158" t="s" s="2">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="AF158" t="s" s="2">
         <v>42</v>
@@ -20300,7 +20291,7 @@
         <v>41</v>
       </c>
       <c r="AK158" t="s" s="2">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="AL158" t="s" s="2">
         <v>41</v>
@@ -20314,7 +20305,7 @@
     </row>
     <row r="159" hidden="true">
       <c r="A159" t="s" s="2">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" t="s" s="2">
@@ -20426,7 +20417,7 @@
     </row>
     <row r="160" hidden="true">
       <c r="A160" t="s" s="2">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" t="s" s="2">
@@ -20540,7 +20531,7 @@
     </row>
     <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" t="s" s="2">
@@ -20654,7 +20645,7 @@
     </row>
     <row r="162" hidden="true">
       <c r="A162" t="s" s="2">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" t="s" s="2">
@@ -20768,7 +20759,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -20882,7 +20873,7 @@
     </row>
     <row r="164">
       <c r="A164" t="s" s="2">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" t="s" s="2">
@@ -20908,10 +20899,10 @@
         <v>52</v>
       </c>
       <c r="K164" t="s" s="2">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="L164" t="s" s="2">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="M164" t="s" s="2">
         <v>204</v>
@@ -20996,7 +20987,7 @@
     </row>
     <row r="165" hidden="true">
       <c r="A165" t="s" s="2">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" t="s" s="2">
@@ -21019,16 +21010,16 @@
         <v>41</v>
       </c>
       <c r="J165" t="s" s="2">
+        <v>676</v>
+      </c>
+      <c r="K165" t="s" s="2">
+        <v>677</v>
+      </c>
+      <c r="L165" t="s" s="2">
+        <v>678</v>
+      </c>
+      <c r="M165" t="s" s="2">
         <v>679</v>
-      </c>
-      <c r="K165" t="s" s="2">
-        <v>680</v>
-      </c>
-      <c r="L165" t="s" s="2">
-        <v>681</v>
-      </c>
-      <c r="M165" t="s" s="2">
-        <v>682</v>
       </c>
       <c r="N165" s="2"/>
       <c r="O165" t="s" s="2">
@@ -21078,7 +21069,7 @@
         <v>41</v>
       </c>
       <c r="AE165" t="s" s="2">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="AF165" t="s" s="2">
         <v>42</v>
@@ -21096,7 +21087,7 @@
         <v>41</v>
       </c>
       <c r="AK165" t="s" s="2">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="AL165" t="s" s="2">
         <v>41</v>

</xml_diff>